<commit_message>
fix bug #118414  #118168
</commit_message>
<xml_diff>
--- a/nts.uk/uk.at/at.file/nts.uk.file.at.infra/src/main/resources/report/KWR003.xlsx
+++ b/nts.uk/uk.at/at.file/nts.uk.file.at.infra/src/main/resources/report/KWR003.xlsx
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" iterateDelta="1E-4"/>
+  <calcPr calcId="124519"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
@@ -20,7 +20,13 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="4">
+  <fonts count="3">
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -29,25 +35,11 @@
     </font>
     <font>
       <sz val="7"/>
-      <color rgb="FF000000"/>
+      <color theme="1"/>
       <name val="ＭＳ ゴシック"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="ＭＳ ゴシック"/>
-      <family val="3"/>
-      <charset val="128"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -56,24 +48,36 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor rgb="FFFFFFCC"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF9BC2E6"/>
+        <fgColor theme="0"/>
         <bgColor rgb="FFC0C0C0"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFDDEBF7"/>
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor rgb="FFC0C0C0"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
         <bgColor rgb="FFCCFFFF"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -164,13 +168,78 @@
     </border>
     <border>
       <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="dotted">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="dotted">
         <color auto="1"/>
       </right>
       <top style="thin">
         <color auto="1"/>
       </top>
-      <bottom style="thin">
+      <bottom style="dotted">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="dotted">
+        <color auto="1"/>
+      </left>
+      <right style="dotted">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="dotted">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="dotted">
+        <color auto="1"/>
+      </top>
+      <bottom style="dotted">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="dotted">
+        <color auto="1"/>
+      </right>
+      <top style="dotted">
+        <color auto="1"/>
+      </top>
+      <bottom style="dotted">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="dotted">
+        <color auto="1"/>
+      </left>
+      <right style="dotted">
+        <color auto="1"/>
+      </right>
+      <top style="dotted">
+        <color auto="1"/>
+      </top>
+      <bottom style="dotted">
         <color auto="1"/>
       </bottom>
       <diagonal/>
@@ -178,61 +247,79 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="3" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="2" fillId="5" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="3" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="2" fillId="5" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="3" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="2" fillId="5" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="3" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="2" fillId="4" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="4" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="2" fillId="6" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="1" fillId="4" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="2" fillId="6" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="4" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="6" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="2" fillId="6" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="5" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="3" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="2" fillId="5" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="3" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="2" fillId="5" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="3" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="2" fillId="4" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="6" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="6" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -609,7 +696,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -617,19 +704,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AJ14"/>
+  <dimension ref="A1:AJ7"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
-    </sheetView>
+    <sheetView tabSelected="1" view="pageLayout" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="3.140625" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="3.85546875" defaultRowHeight="13.5" customHeight="1"/>
   <cols>
-    <col min="1" max="3" width="2.5703125" customWidth="1"/>
-    <col min="36" max="36" width="2.7109375" customWidth="1"/>
+    <col min="1" max="1" width="1.42578125" style="8" customWidth="1"/>
+    <col min="2" max="3" width="3.42578125" style="8" customWidth="1"/>
+    <col min="4" max="16384" width="3.85546875" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36">
+    <row r="1" spans="1:36" ht="13.5" customHeight="1">
       <c r="A1" s="1"/>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -667,10 +753,10 @@
       <c r="AI1" s="3"/>
       <c r="AJ1" s="3"/>
     </row>
-    <row r="2" spans="1:36">
-      <c r="A2" s="13"/>
-      <c r="B2" s="13"/>
-      <c r="C2" s="13"/>
+    <row r="2" spans="1:36" ht="13.5" customHeight="1">
+      <c r="A2" s="15"/>
+      <c r="B2" s="15"/>
+      <c r="C2" s="15"/>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
       <c r="F2" s="4"/>
@@ -702,13 +788,13 @@
       <c r="AF2" s="4"/>
       <c r="AG2" s="4"/>
       <c r="AH2" s="4"/>
-      <c r="AI2" s="14"/>
-      <c r="AJ2" s="14"/>
+      <c r="AI2" s="16"/>
+      <c r="AJ2" s="16"/>
     </row>
-    <row r="3" spans="1:36">
-      <c r="A3" s="13"/>
-      <c r="B3" s="13"/>
-      <c r="C3" s="13"/>
+    <row r="3" spans="1:36" ht="13.5" customHeight="1">
+      <c r="A3" s="15"/>
+      <c r="B3" s="15"/>
+      <c r="C3" s="15"/>
       <c r="D3" s="5"/>
       <c r="E3" s="5"/>
       <c r="F3" s="5"/>
@@ -740,177 +826,174 @@
       <c r="AF3" s="5"/>
       <c r="AG3" s="5"/>
       <c r="AH3" s="5"/>
-      <c r="AI3" s="14"/>
-      <c r="AJ3" s="14"/>
+      <c r="AI3" s="16"/>
+      <c r="AJ3" s="16"/>
     </row>
-    <row r="4" spans="1:36">
-      <c r="A4" s="15"/>
-      <c r="B4" s="15"/>
-      <c r="C4" s="15"/>
-      <c r="D4" s="15"/>
-      <c r="E4" s="15"/>
-      <c r="F4" s="15"/>
-      <c r="G4" s="15"/>
-      <c r="H4" s="15"/>
-      <c r="I4" s="15"/>
-      <c r="J4" s="15"/>
-      <c r="K4" s="15"/>
-      <c r="L4" s="15"/>
-      <c r="M4" s="15"/>
-      <c r="N4" s="15"/>
-      <c r="O4" s="15"/>
-      <c r="P4" s="15"/>
-      <c r="Q4" s="15"/>
-      <c r="R4" s="15"/>
-      <c r="S4" s="15"/>
-      <c r="T4" s="15"/>
-      <c r="U4" s="15"/>
-      <c r="V4" s="15"/>
-      <c r="W4" s="15"/>
-      <c r="X4" s="15"/>
-      <c r="Y4" s="15"/>
-      <c r="Z4" s="15"/>
-      <c r="AA4" s="15"/>
-      <c r="AB4" s="15"/>
-      <c r="AC4" s="15"/>
-      <c r="AD4" s="15"/>
-      <c r="AE4" s="15"/>
-      <c r="AF4" s="15"/>
-      <c r="AG4" s="15"/>
-      <c r="AH4" s="15"/>
+    <row r="4" spans="1:36" ht="13.5" customHeight="1">
+      <c r="A4" s="17"/>
+      <c r="B4" s="17"/>
+      <c r="C4" s="17"/>
+      <c r="D4" s="17"/>
+      <c r="E4" s="17"/>
+      <c r="F4" s="17"/>
+      <c r="G4" s="17"/>
+      <c r="H4" s="17"/>
+      <c r="I4" s="17"/>
+      <c r="J4" s="17"/>
+      <c r="K4" s="17"/>
+      <c r="L4" s="17"/>
+      <c r="M4" s="17"/>
+      <c r="N4" s="17"/>
+      <c r="O4" s="17"/>
+      <c r="P4" s="17"/>
+      <c r="Q4" s="17"/>
+      <c r="R4" s="17"/>
+      <c r="S4" s="17"/>
+      <c r="T4" s="17"/>
+      <c r="U4" s="17"/>
+      <c r="V4" s="17"/>
+      <c r="W4" s="17"/>
+      <c r="X4" s="17"/>
+      <c r="Y4" s="17"/>
+      <c r="Z4" s="17"/>
+      <c r="AA4" s="17"/>
+      <c r="AB4" s="17"/>
+      <c r="AC4" s="17"/>
+      <c r="AD4" s="17"/>
+      <c r="AE4" s="17"/>
+      <c r="AF4" s="17"/>
+      <c r="AG4" s="17"/>
+      <c r="AH4" s="17"/>
       <c r="AI4" s="6"/>
       <c r="AJ4" s="6"/>
     </row>
-    <row r="5" spans="1:36">
-      <c r="A5" s="16"/>
-      <c r="B5" s="16"/>
-      <c r="C5" s="16"/>
-      <c r="D5" s="16"/>
-      <c r="E5" s="16"/>
-      <c r="F5" s="16"/>
-      <c r="G5" s="16"/>
-      <c r="H5" s="16"/>
-      <c r="I5" s="16"/>
-      <c r="J5" s="16"/>
-      <c r="K5" s="16"/>
-      <c r="L5" s="16"/>
-      <c r="M5" s="16"/>
-      <c r="N5" s="16"/>
-      <c r="O5" s="16"/>
-      <c r="P5" s="16"/>
-      <c r="Q5" s="16"/>
-      <c r="R5" s="16"/>
-      <c r="S5" s="16"/>
-      <c r="T5" s="16"/>
-      <c r="U5" s="16"/>
-      <c r="V5" s="16"/>
-      <c r="W5" s="16"/>
-      <c r="X5" s="16"/>
-      <c r="Y5" s="16"/>
-      <c r="Z5" s="16"/>
-      <c r="AA5" s="16"/>
-      <c r="AB5" s="16"/>
-      <c r="AC5" s="16"/>
-      <c r="AD5" s="16"/>
-      <c r="AE5" s="16"/>
-      <c r="AF5" s="16"/>
-      <c r="AG5" s="16"/>
-      <c r="AH5" s="16"/>
+    <row r="5" spans="1:36" ht="13.5" customHeight="1">
+      <c r="A5" s="18"/>
+      <c r="B5" s="18"/>
+      <c r="C5" s="18"/>
+      <c r="D5" s="18"/>
+      <c r="E5" s="18"/>
+      <c r="F5" s="18"/>
+      <c r="G5" s="18"/>
+      <c r="H5" s="18"/>
+      <c r="I5" s="18"/>
+      <c r="J5" s="18"/>
+      <c r="K5" s="18"/>
+      <c r="L5" s="18"/>
+      <c r="M5" s="18"/>
+      <c r="N5" s="18"/>
+      <c r="O5" s="18"/>
+      <c r="P5" s="18"/>
+      <c r="Q5" s="18"/>
+      <c r="R5" s="18"/>
+      <c r="S5" s="18"/>
+      <c r="T5" s="18"/>
+      <c r="U5" s="18"/>
+      <c r="V5" s="18"/>
+      <c r="W5" s="18"/>
+      <c r="X5" s="18"/>
+      <c r="Y5" s="18"/>
+      <c r="Z5" s="18"/>
+      <c r="AA5" s="18"/>
+      <c r="AB5" s="18"/>
+      <c r="AC5" s="18"/>
+      <c r="AD5" s="18"/>
+      <c r="AE5" s="18"/>
+      <c r="AF5" s="18"/>
+      <c r="AG5" s="18"/>
+      <c r="AH5" s="18"/>
       <c r="AI5" s="7"/>
       <c r="AJ5" s="7"/>
     </row>
-    <row r="6" spans="1:36">
-      <c r="A6" s="17"/>
-      <c r="B6" s="17"/>
-      <c r="C6" s="17"/>
-      <c r="D6" s="8"/>
-      <c r="E6" s="8"/>
-      <c r="F6" s="8"/>
-      <c r="G6" s="8"/>
-      <c r="H6" s="8"/>
-      <c r="I6" s="8"/>
-      <c r="J6" s="8"/>
-      <c r="K6" s="8"/>
-      <c r="L6" s="8"/>
-      <c r="M6" s="8"/>
-      <c r="N6" s="8"/>
-      <c r="O6" s="8"/>
-      <c r="P6" s="8"/>
-      <c r="Q6" s="8"/>
-      <c r="R6" s="8"/>
-      <c r="S6" s="8"/>
-      <c r="T6" s="8"/>
-      <c r="U6" s="8"/>
-      <c r="V6" s="8"/>
-      <c r="W6" s="8"/>
-      <c r="X6" s="8"/>
-      <c r="Y6" s="8"/>
-      <c r="Z6" s="8"/>
-      <c r="AA6" s="8"/>
-      <c r="AB6" s="8"/>
-      <c r="AC6" s="8"/>
-      <c r="AD6" s="8"/>
-      <c r="AE6" s="8"/>
-      <c r="AF6" s="8"/>
-      <c r="AG6" s="8"/>
-      <c r="AH6" s="8"/>
-      <c r="AI6" s="18"/>
-      <c r="AJ6" s="18"/>
+    <row r="6" spans="1:36" ht="13.5" customHeight="1">
+      <c r="A6" s="12"/>
+      <c r="B6" s="21"/>
+      <c r="C6" s="22"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="9"/>
+      <c r="G6" s="9"/>
+      <c r="H6" s="9"/>
+      <c r="I6" s="9"/>
+      <c r="J6" s="9"/>
+      <c r="K6" s="9"/>
+      <c r="L6" s="9"/>
+      <c r="M6" s="9"/>
+      <c r="N6" s="9"/>
+      <c r="O6" s="9"/>
+      <c r="P6" s="9"/>
+      <c r="Q6" s="9"/>
+      <c r="R6" s="9"/>
+      <c r="S6" s="9"/>
+      <c r="T6" s="9"/>
+      <c r="U6" s="9"/>
+      <c r="V6" s="9"/>
+      <c r="W6" s="9"/>
+      <c r="X6" s="9"/>
+      <c r="Y6" s="9"/>
+      <c r="Z6" s="9"/>
+      <c r="AA6" s="9"/>
+      <c r="AB6" s="9"/>
+      <c r="AC6" s="9"/>
+      <c r="AD6" s="9"/>
+      <c r="AE6" s="9"/>
+      <c r="AF6" s="9"/>
+      <c r="AG6" s="9"/>
+      <c r="AH6" s="9"/>
+      <c r="AI6" s="19"/>
+      <c r="AJ6" s="20"/>
     </row>
-    <row r="7" spans="1:36">
+    <row r="7" spans="1:36" ht="13.5" customHeight="1">
       <c r="A7" s="11"/>
-      <c r="B7" s="11"/>
-      <c r="C7" s="11"/>
-      <c r="D7" s="9"/>
-      <c r="E7" s="9"/>
-      <c r="F7" s="9"/>
-      <c r="G7" s="9"/>
-      <c r="H7" s="9"/>
-      <c r="I7" s="9"/>
-      <c r="J7" s="9"/>
-      <c r="K7" s="9"/>
-      <c r="L7" s="9"/>
-      <c r="M7" s="9"/>
-      <c r="N7" s="9"/>
-      <c r="O7" s="9"/>
-      <c r="P7" s="9"/>
-      <c r="Q7" s="9"/>
-      <c r="R7" s="9"/>
-      <c r="S7" s="9"/>
-      <c r="T7" s="9"/>
-      <c r="U7" s="9"/>
-      <c r="V7" s="9"/>
-      <c r="W7" s="9"/>
-      <c r="X7" s="9"/>
-      <c r="Y7" s="9"/>
-      <c r="Z7" s="9"/>
-      <c r="AA7" s="9"/>
-      <c r="AB7" s="9"/>
-      <c r="AC7" s="9"/>
-      <c r="AD7" s="9"/>
-      <c r="AE7" s="9"/>
-      <c r="AF7" s="9"/>
-      <c r="AG7" s="9"/>
-      <c r="AH7" s="9"/>
-      <c r="AI7" s="12"/>
-      <c r="AJ7" s="12"/>
-    </row>
-    <row r="14" spans="1:36">
-      <c r="G14" s="10"/>
+      <c r="B7" s="23"/>
+      <c r="C7" s="24"/>
+      <c r="D7" s="10"/>
+      <c r="E7" s="10"/>
+      <c r="F7" s="10"/>
+      <c r="G7" s="10"/>
+      <c r="H7" s="10"/>
+      <c r="I7" s="10"/>
+      <c r="J7" s="10"/>
+      <c r="K7" s="10"/>
+      <c r="L7" s="10"/>
+      <c r="M7" s="10"/>
+      <c r="N7" s="10"/>
+      <c r="O7" s="10"/>
+      <c r="P7" s="10"/>
+      <c r="Q7" s="10"/>
+      <c r="R7" s="10"/>
+      <c r="S7" s="10"/>
+      <c r="T7" s="10"/>
+      <c r="U7" s="10"/>
+      <c r="V7" s="10"/>
+      <c r="W7" s="10"/>
+      <c r="X7" s="10"/>
+      <c r="Y7" s="10"/>
+      <c r="Z7" s="10"/>
+      <c r="AA7" s="10"/>
+      <c r="AB7" s="10"/>
+      <c r="AC7" s="10"/>
+      <c r="AD7" s="10"/>
+      <c r="AE7" s="10"/>
+      <c r="AF7" s="10"/>
+      <c r="AG7" s="10"/>
+      <c r="AH7" s="10"/>
+      <c r="AI7" s="13"/>
+      <c r="AJ7" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="8">
-    <mergeCell ref="A7:C7"/>
     <mergeCell ref="AI7:AJ7"/>
     <mergeCell ref="A2:C3"/>
     <mergeCell ref="AI2:AJ3"/>
     <mergeCell ref="A4:AH4"/>
     <mergeCell ref="A5:AH5"/>
-    <mergeCell ref="A6:C6"/>
     <mergeCell ref="AI6:AJ6"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B7:C7"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
-  <pageMargins left="1" right="1.5" top="1.5" bottom="1.5" header="0.8" footer="0.8"/>
-  <pageSetup orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageMargins left="0.39370078740157483" right="0.39370078740157483" top="0.78740157480314965" bottom="0.39370078740157483" header="0.31496062992125984" footer="0.31496062992125984"/>
+  <pageSetup paperSize="9" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fix bug  #118414   # 118168
</commit_message>
<xml_diff>
--- a/nts.uk/uk.at/at.file/nts.uk.file.at.infra/src/main/resources/report/KWR003.xlsx
+++ b/nts.uk/uk.at/at.file/nts.uk.file.at.infra/src/main/resources/report/KWR003.xlsx
@@ -77,7 +77,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -160,8 +160,38 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="thin">
+      <top style="dotted">
+        <color auto="1"/>
+      </top>
+      <bottom style="dotted">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="dotted">
+        <color auto="1"/>
+      </right>
+      <top style="dotted">
+        <color auto="1"/>
+      </top>
+      <bottom style="dotted">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="dotted">
+        <color auto="1"/>
+      </left>
+      <right style="dotted">
+        <color auto="1"/>
+      </right>
+      <top style="dotted">
+        <color auto="1"/>
+      </top>
+      <bottom style="dotted">
         <color auto="1"/>
       </bottom>
       <diagonal/>
@@ -169,9 +199,7 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
+      <top/>
       <bottom style="dotted">
         <color auto="1"/>
       </bottom>
@@ -182,9 +210,7 @@
       <right style="dotted">
         <color auto="1"/>
       </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
+      <top/>
       <bottom style="dotted">
         <color auto="1"/>
       </bottom>
@@ -197,48 +223,7 @@
       <right style="dotted">
         <color auto="1"/>
       </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="dotted">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="dotted">
-        <color auto="1"/>
-      </top>
-      <bottom style="dotted">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="dotted">
-        <color auto="1"/>
-      </right>
-      <top style="dotted">
-        <color auto="1"/>
-      </top>
-      <bottom style="dotted">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="dotted">
-        <color auto="1"/>
-      </left>
-      <right style="dotted">
-        <color auto="1"/>
-      </right>
-      <top style="dotted">
-        <color auto="1"/>
-      </top>
+      <top/>
       <bottom style="dotted">
         <color auto="1"/>
       </bottom>
@@ -249,7 +234,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
@@ -269,26 +254,50 @@
     <xf numFmtId="49" fontId="2" fillId="5" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="4" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="2" fillId="6" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="6" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="6" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="4" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="6" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="6" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="2" fillId="6" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="2" fillId="6" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="6" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="2" fillId="6" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="6" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="2" fillId="6" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="5" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -300,26 +309,8 @@
     <xf numFmtId="49" fontId="2" fillId="5" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="4" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="2" fillId="4" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="6" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="6" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -704,15 +695,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AJ7"/>
+  <dimension ref="A1:AJ9"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" workbookViewId="0"/>
+    <sheetView tabSelected="1" view="pageLayout" zoomScale="115" zoomScalePageLayoutView="115" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.85546875" defaultRowHeight="13.5" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="1.42578125" style="8" customWidth="1"/>
-    <col min="2" max="3" width="3.42578125" style="8" customWidth="1"/>
-    <col min="4" max="16384" width="3.85546875" style="8"/>
+    <col min="1" max="1" width="1.42578125" style="7" customWidth="1"/>
+    <col min="2" max="3" width="3.42578125" style="7" customWidth="1"/>
+    <col min="4" max="16384" width="3.85546875" style="7"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:36" ht="13.5" customHeight="1">
@@ -754,9 +745,9 @@
       <c r="AJ1" s="3"/>
     </row>
     <row r="2" spans="1:36" ht="13.5" customHeight="1">
-      <c r="A2" s="15"/>
-      <c r="B2" s="15"/>
-      <c r="C2" s="15"/>
+      <c r="A2" s="23"/>
+      <c r="B2" s="23"/>
+      <c r="C2" s="23"/>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
       <c r="F2" s="4"/>
@@ -788,13 +779,13 @@
       <c r="AF2" s="4"/>
       <c r="AG2" s="4"/>
       <c r="AH2" s="4"/>
-      <c r="AI2" s="16"/>
-      <c r="AJ2" s="16"/>
+      <c r="AI2" s="24"/>
+      <c r="AJ2" s="24"/>
     </row>
     <row r="3" spans="1:36" ht="13.5" customHeight="1">
-      <c r="A3" s="15"/>
-      <c r="B3" s="15"/>
-      <c r="C3" s="15"/>
+      <c r="A3" s="23"/>
+      <c r="B3" s="23"/>
+      <c r="C3" s="23"/>
       <c r="D3" s="5"/>
       <c r="E3" s="5"/>
       <c r="F3" s="5"/>
@@ -826,170 +817,250 @@
       <c r="AF3" s="5"/>
       <c r="AG3" s="5"/>
       <c r="AH3" s="5"/>
-      <c r="AI3" s="16"/>
-      <c r="AJ3" s="16"/>
+      <c r="AI3" s="24"/>
+      <c r="AJ3" s="24"/>
     </row>
-    <row r="4" spans="1:36" ht="13.5" customHeight="1">
-      <c r="A4" s="17"/>
-      <c r="B4" s="17"/>
-      <c r="C4" s="17"/>
-      <c r="D4" s="17"/>
-      <c r="E4" s="17"/>
-      <c r="F4" s="17"/>
-      <c r="G4" s="17"/>
-      <c r="H4" s="17"/>
-      <c r="I4" s="17"/>
-      <c r="J4" s="17"/>
-      <c r="K4" s="17"/>
-      <c r="L4" s="17"/>
-      <c r="M4" s="17"/>
-      <c r="N4" s="17"/>
-      <c r="O4" s="17"/>
-      <c r="P4" s="17"/>
-      <c r="Q4" s="17"/>
-      <c r="R4" s="17"/>
-      <c r="S4" s="17"/>
-      <c r="T4" s="17"/>
-      <c r="U4" s="17"/>
-      <c r="V4" s="17"/>
-      <c r="W4" s="17"/>
-      <c r="X4" s="17"/>
-      <c r="Y4" s="17"/>
-      <c r="Z4" s="17"/>
-      <c r="AA4" s="17"/>
-      <c r="AB4" s="17"/>
-      <c r="AC4" s="17"/>
-      <c r="AD4" s="17"/>
-      <c r="AE4" s="17"/>
-      <c r="AF4" s="17"/>
-      <c r="AG4" s="17"/>
-      <c r="AH4" s="17"/>
+    <row r="4" spans="1:36" ht="13.5" customHeight="1" thickBot="1">
+      <c r="A4" s="25"/>
+      <c r="B4" s="25"/>
+      <c r="C4" s="25"/>
+      <c r="D4" s="25"/>
+      <c r="E4" s="25"/>
+      <c r="F4" s="25"/>
+      <c r="G4" s="25"/>
+      <c r="H4" s="25"/>
+      <c r="I4" s="25"/>
+      <c r="J4" s="25"/>
+      <c r="K4" s="25"/>
+      <c r="L4" s="25"/>
+      <c r="M4" s="25"/>
+      <c r="N4" s="25"/>
+      <c r="O4" s="25"/>
+      <c r="P4" s="25"/>
+      <c r="Q4" s="25"/>
+      <c r="R4" s="25"/>
+      <c r="S4" s="25"/>
+      <c r="T4" s="25"/>
+      <c r="U4" s="25"/>
+      <c r="V4" s="25"/>
+      <c r="W4" s="25"/>
+      <c r="X4" s="25"/>
+      <c r="Y4" s="25"/>
+      <c r="Z4" s="25"/>
+      <c r="AA4" s="25"/>
+      <c r="AB4" s="25"/>
+      <c r="AC4" s="25"/>
+      <c r="AD4" s="25"/>
+      <c r="AE4" s="25"/>
+      <c r="AF4" s="25"/>
+      <c r="AG4" s="25"/>
+      <c r="AH4" s="25"/>
       <c r="AI4" s="6"/>
       <c r="AJ4" s="6"/>
     </row>
-    <row r="5" spans="1:36" ht="13.5" customHeight="1">
-      <c r="A5" s="18"/>
-      <c r="B5" s="18"/>
-      <c r="C5" s="18"/>
-      <c r="D5" s="18"/>
-      <c r="E5" s="18"/>
-      <c r="F5" s="18"/>
-      <c r="G5" s="18"/>
-      <c r="H5" s="18"/>
-      <c r="I5" s="18"/>
-      <c r="J5" s="18"/>
-      <c r="K5" s="18"/>
-      <c r="L5" s="18"/>
-      <c r="M5" s="18"/>
-      <c r="N5" s="18"/>
-      <c r="O5" s="18"/>
-      <c r="P5" s="18"/>
-      <c r="Q5" s="18"/>
-      <c r="R5" s="18"/>
-      <c r="S5" s="18"/>
-      <c r="T5" s="18"/>
-      <c r="U5" s="18"/>
-      <c r="V5" s="18"/>
-      <c r="W5" s="18"/>
-      <c r="X5" s="18"/>
-      <c r="Y5" s="18"/>
-      <c r="Z5" s="18"/>
-      <c r="AA5" s="18"/>
-      <c r="AB5" s="18"/>
-      <c r="AC5" s="18"/>
-      <c r="AD5" s="18"/>
-      <c r="AE5" s="18"/>
-      <c r="AF5" s="18"/>
-      <c r="AG5" s="18"/>
-      <c r="AH5" s="18"/>
-      <c r="AI5" s="7"/>
-      <c r="AJ5" s="7"/>
+    <row r="5" spans="1:36" ht="13.5" customHeight="1" thickBot="1">
+      <c r="A5" s="26"/>
+      <c r="B5" s="26"/>
+      <c r="C5" s="26"/>
+      <c r="D5" s="26"/>
+      <c r="E5" s="26"/>
+      <c r="F5" s="26"/>
+      <c r="G5" s="26"/>
+      <c r="H5" s="26"/>
+      <c r="I5" s="26"/>
+      <c r="J5" s="26"/>
+      <c r="K5" s="26"/>
+      <c r="L5" s="26"/>
+      <c r="M5" s="26"/>
+      <c r="N5" s="26"/>
+      <c r="O5" s="26"/>
+      <c r="P5" s="26"/>
+      <c r="Q5" s="26"/>
+      <c r="R5" s="26"/>
+      <c r="S5" s="26"/>
+      <c r="T5" s="26"/>
+      <c r="U5" s="26"/>
+      <c r="V5" s="26"/>
+      <c r="W5" s="26"/>
+      <c r="X5" s="26"/>
+      <c r="Y5" s="26"/>
+      <c r="Z5" s="26"/>
+      <c r="AA5" s="26"/>
+      <c r="AB5" s="26"/>
+      <c r="AC5" s="26"/>
+      <c r="AD5" s="26"/>
+      <c r="AE5" s="26"/>
+      <c r="AF5" s="26"/>
+      <c r="AG5" s="26"/>
+      <c r="AH5" s="26"/>
+      <c r="AI5" s="14"/>
+      <c r="AJ5" s="14"/>
     </row>
     <row r="6" spans="1:36" ht="13.5" customHeight="1">
-      <c r="A6" s="12"/>
-      <c r="B6" s="21"/>
-      <c r="C6" s="22"/>
-      <c r="D6" s="9"/>
-      <c r="E6" s="9"/>
-      <c r="F6" s="9"/>
-      <c r="G6" s="9"/>
-      <c r="H6" s="9"/>
-      <c r="I6" s="9"/>
-      <c r="J6" s="9"/>
-      <c r="K6" s="9"/>
-      <c r="L6" s="9"/>
-      <c r="M6" s="9"/>
-      <c r="N6" s="9"/>
-      <c r="O6" s="9"/>
-      <c r="P6" s="9"/>
-      <c r="Q6" s="9"/>
-      <c r="R6" s="9"/>
-      <c r="S6" s="9"/>
-      <c r="T6" s="9"/>
-      <c r="U6" s="9"/>
-      <c r="V6" s="9"/>
-      <c r="W6" s="9"/>
-      <c r="X6" s="9"/>
-      <c r="Y6" s="9"/>
-      <c r="Z6" s="9"/>
-      <c r="AA6" s="9"/>
-      <c r="AB6" s="9"/>
-      <c r="AC6" s="9"/>
-      <c r="AD6" s="9"/>
-      <c r="AE6" s="9"/>
-      <c r="AF6" s="9"/>
-      <c r="AG6" s="9"/>
-      <c r="AH6" s="9"/>
-      <c r="AI6" s="19"/>
-      <c r="AJ6" s="20"/>
+      <c r="A6" s="10"/>
+      <c r="B6" s="15"/>
+      <c r="C6" s="16"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="11"/>
+      <c r="F6" s="11"/>
+      <c r="G6" s="11"/>
+      <c r="H6" s="11"/>
+      <c r="I6" s="11"/>
+      <c r="J6" s="11"/>
+      <c r="K6" s="11"/>
+      <c r="L6" s="11"/>
+      <c r="M6" s="11"/>
+      <c r="N6" s="11"/>
+      <c r="O6" s="11"/>
+      <c r="P6" s="11"/>
+      <c r="Q6" s="11"/>
+      <c r="R6" s="11"/>
+      <c r="S6" s="11"/>
+      <c r="T6" s="11"/>
+      <c r="U6" s="11"/>
+      <c r="V6" s="11"/>
+      <c r="W6" s="11"/>
+      <c r="X6" s="11"/>
+      <c r="Y6" s="11"/>
+      <c r="Z6" s="11"/>
+      <c r="AA6" s="11"/>
+      <c r="AB6" s="11"/>
+      <c r="AC6" s="11"/>
+      <c r="AD6" s="11"/>
+      <c r="AE6" s="11"/>
+      <c r="AF6" s="11"/>
+      <c r="AG6" s="11"/>
+      <c r="AH6" s="11"/>
+      <c r="AI6" s="17"/>
+      <c r="AJ6" s="18"/>
     </row>
     <row r="7" spans="1:36" ht="13.5" customHeight="1">
-      <c r="A7" s="11"/>
-      <c r="B7" s="23"/>
-      <c r="C7" s="24"/>
-      <c r="D7" s="10"/>
-      <c r="E7" s="10"/>
-      <c r="F7" s="10"/>
-      <c r="G7" s="10"/>
-      <c r="H7" s="10"/>
-      <c r="I7" s="10"/>
-      <c r="J7" s="10"/>
-      <c r="K7" s="10"/>
-      <c r="L7" s="10"/>
-      <c r="M7" s="10"/>
-      <c r="N7" s="10"/>
-      <c r="O7" s="10"/>
-      <c r="P7" s="10"/>
-      <c r="Q7" s="10"/>
-      <c r="R7" s="10"/>
-      <c r="S7" s="10"/>
-      <c r="T7" s="10"/>
-      <c r="U7" s="10"/>
-      <c r="V7" s="10"/>
-      <c r="W7" s="10"/>
-      <c r="X7" s="10"/>
-      <c r="Y7" s="10"/>
-      <c r="Z7" s="10"/>
-      <c r="AA7" s="10"/>
-      <c r="AB7" s="10"/>
-      <c r="AC7" s="10"/>
-      <c r="AD7" s="10"/>
-      <c r="AE7" s="10"/>
-      <c r="AF7" s="10"/>
-      <c r="AG7" s="10"/>
-      <c r="AH7" s="10"/>
-      <c r="AI7" s="13"/>
-      <c r="AJ7" s="14"/>
+      <c r="A7" s="9"/>
+      <c r="B7" s="19"/>
+      <c r="C7" s="20"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="8"/>
+      <c r="G7" s="8"/>
+      <c r="H7" s="8"/>
+      <c r="I7" s="8"/>
+      <c r="J7" s="8"/>
+      <c r="K7" s="8"/>
+      <c r="L7" s="8"/>
+      <c r="M7" s="8"/>
+      <c r="N7" s="8"/>
+      <c r="O7" s="8"/>
+      <c r="P7" s="8"/>
+      <c r="Q7" s="8"/>
+      <c r="R7" s="8"/>
+      <c r="S7" s="8"/>
+      <c r="T7" s="8"/>
+      <c r="U7" s="8"/>
+      <c r="V7" s="8"/>
+      <c r="W7" s="8"/>
+      <c r="X7" s="8"/>
+      <c r="Y7" s="8"/>
+      <c r="Z7" s="8"/>
+      <c r="AA7" s="8"/>
+      <c r="AB7" s="8"/>
+      <c r="AC7" s="8"/>
+      <c r="AD7" s="8"/>
+      <c r="AE7" s="8"/>
+      <c r="AF7" s="8"/>
+      <c r="AG7" s="8"/>
+      <c r="AH7" s="8"/>
+      <c r="AI7" s="21"/>
+      <c r="AJ7" s="22"/>
+    </row>
+    <row r="8" spans="1:36" ht="13.5" customHeight="1">
+      <c r="A8" s="12"/>
+      <c r="B8" s="15"/>
+      <c r="C8" s="16"/>
+      <c r="D8" s="11"/>
+      <c r="E8" s="11"/>
+      <c r="F8" s="11"/>
+      <c r="G8" s="11"/>
+      <c r="H8" s="11"/>
+      <c r="I8" s="11"/>
+      <c r="J8" s="11"/>
+      <c r="K8" s="11"/>
+      <c r="L8" s="11"/>
+      <c r="M8" s="11"/>
+      <c r="N8" s="11"/>
+      <c r="O8" s="11"/>
+      <c r="P8" s="11"/>
+      <c r="Q8" s="11"/>
+      <c r="R8" s="11"/>
+      <c r="S8" s="11"/>
+      <c r="T8" s="11"/>
+      <c r="U8" s="11"/>
+      <c r="V8" s="11"/>
+      <c r="W8" s="11"/>
+      <c r="X8" s="11"/>
+      <c r="Y8" s="11"/>
+      <c r="Z8" s="11"/>
+      <c r="AA8" s="11"/>
+      <c r="AB8" s="11"/>
+      <c r="AC8" s="11"/>
+      <c r="AD8" s="11"/>
+      <c r="AE8" s="11"/>
+      <c r="AF8" s="11"/>
+      <c r="AG8" s="11"/>
+      <c r="AH8" s="11"/>
+      <c r="AI8" s="17"/>
+      <c r="AJ8" s="18"/>
+    </row>
+    <row r="9" spans="1:36" ht="13.5" customHeight="1">
+      <c r="A9" s="13"/>
+      <c r="B9" s="19"/>
+      <c r="C9" s="20"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="8"/>
+      <c r="G9" s="8"/>
+      <c r="H9" s="8"/>
+      <c r="I9" s="8"/>
+      <c r="J9" s="8"/>
+      <c r="K9" s="8"/>
+      <c r="L9" s="8"/>
+      <c r="M9" s="8"/>
+      <c r="N9" s="8"/>
+      <c r="O9" s="8"/>
+      <c r="P9" s="8"/>
+      <c r="Q9" s="8"/>
+      <c r="R9" s="8"/>
+      <c r="S9" s="8"/>
+      <c r="T9" s="8"/>
+      <c r="U9" s="8"/>
+      <c r="V9" s="8"/>
+      <c r="W9" s="8"/>
+      <c r="X9" s="8"/>
+      <c r="Y9" s="8"/>
+      <c r="Z9" s="8"/>
+      <c r="AA9" s="8"/>
+      <c r="AB9" s="8"/>
+      <c r="AC9" s="8"/>
+      <c r="AD9" s="8"/>
+      <c r="AE9" s="8"/>
+      <c r="AF9" s="8"/>
+      <c r="AG9" s="8"/>
+      <c r="AH9" s="8"/>
+      <c r="AI9" s="21"/>
+      <c r="AJ9" s="22"/>
     </row>
   </sheetData>
-  <mergeCells count="8">
-    <mergeCell ref="AI7:AJ7"/>
+  <mergeCells count="12">
     <mergeCell ref="A2:C3"/>
     <mergeCell ref="AI2:AJ3"/>
     <mergeCell ref="A4:AH4"/>
     <mergeCell ref="A5:AH5"/>
     <mergeCell ref="AI6:AJ6"/>
     <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="AI8:AJ8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="AI9:AJ9"/>
+    <mergeCell ref="AI7:AJ7"/>
     <mergeCell ref="B7:C7"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>

</xml_diff>